<commit_message>
Verify Valid login test
</commit_message>
<xml_diff>
--- a/src/main/resources/data/test_data.xlsx
+++ b/src/main/resources/data/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INT\westpac\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5584EB-5B9D-4F0E-883F-E5782D1E1AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE0C7CD-C32B-4663-8C07-EC357C5F9825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34512" yWindow="3288" windowWidth="21600" windowHeight="11292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -37,13 +37,19 @@
     <t>Type</t>
   </si>
   <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>A@1234T</t>
-  </si>
-  <si>
     <t>Vaild</t>
+  </si>
+  <si>
+    <t>Login1</t>
+  </si>
+  <si>
+    <t>Pwd@abcd1</t>
+  </si>
+  <si>
+    <t>Fname1</t>
+  </si>
+  <si>
+    <t>FirstName</t>
   </si>
 </sst>
 </file>
@@ -386,15 +392,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,18 +411,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verify Invalid login test
</commit_message>
<xml_diff>
--- a/src/main/resources/data/test_data.xlsx
+++ b/src/main/resources/data/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INT\westpac\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE0C7CD-C32B-4663-8C07-EC357C5F9825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D23B79D-5635-4761-9E8F-1877F1DB64D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34512" yWindow="3288" windowWidth="21600" windowHeight="11292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30984" yWindow="2700" windowWidth="21600" windowHeight="11292" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
     <sheet name="Valid_Login" sheetId="1" r:id="rId2"/>
+    <sheet name="Invalid_Login" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>UserName</t>
   </si>
@@ -50,6 +51,24 @@
   </si>
   <si>
     <t>FirstName</t>
+  </si>
+  <si>
+    <t>LoginX</t>
+  </si>
+  <si>
+    <t>invalidLoginName</t>
+  </si>
+  <si>
+    <t>NullLoginName</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>NullPwd</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -94,9 +113,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -394,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,4 +457,67 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D0D358-DBF1-4EC2-8884-FCA99CFBD1AD}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{59AC14EC-7F98-4435-8897-4B230BF7FAA0}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{4382DE64-0686-4BF1-894C-E894478F249D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Register New user Field test
</commit_message>
<xml_diff>
--- a/src/main/resources/data/test_data.xlsx
+++ b/src/main/resources/data/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INT\westpac\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D23B79D-5635-4761-9E8F-1877F1DB64D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2761DC-C2D8-4735-983D-6AC956EF99FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30984" yWindow="2700" windowWidth="21600" windowHeight="11292" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
     <sheet name="Valid_Login" sheetId="1" r:id="rId2"/>
     <sheet name="Invalid_Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Register_User" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>UserName</t>
   </si>
@@ -69,6 +70,33 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>Pwd</t>
+  </si>
+  <si>
+    <t>ConfirmPwd</t>
+  </si>
+  <si>
+    <t>UserA01</t>
+  </si>
+  <si>
+    <t>FnameA</t>
+  </si>
+  <si>
+    <t>LnameB</t>
+  </si>
+  <si>
+    <t>Pwd@123</t>
   </si>
 </sst>
 </file>
@@ -463,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D0D358-DBF1-4EC2-8884-FCA99CFBD1AD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -520,4 +548,57 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8573CC-FCB9-454B-9583-0F919C825ACD}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B99E95ED-254C-47D0-8999-5C7EBFC7CE59}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{31DD77E4-1160-401D-827A-7ECD19A560CD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>